<commit_message>
Added, split window, hand wave motion detection and UI improvements
</commit_message>
<xml_diff>
--- a/project/messages.xlsx
+++ b/project/messages.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Omkaar\Desktop\Projects\avatar-project\project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5059E61-69C3-45AF-A60C-DAD7FCABA859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D00EE106-92FC-4631-BF2A-4170CBDE2D6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,19 +25,19 @@
     <t>message</t>
   </si>
   <si>
-    <t>Welcome to Christ University. Thanks for joining the Corporate Conclave by the School of Sciences. We are happy to have you today. You can check the agenda for today on the left</t>
-  </si>
-  <si>
-    <t>A warm welcome to the School of Sciences Corporate Conclave. Thank you for being part of this gathering. You can check the agenda for today on the left</t>
-  </si>
-  <si>
-    <t>We are honored to welcome you to the Christ University Corporate Conclave. Your presence enriches our event. You can check the agenda for today on the left</t>
-  </si>
-  <si>
-    <t>Greetings! We are delighted to have you join us for today's Corporate Conclave at Christ University. You can check the agenda for today on the left</t>
-  </si>
-  <si>
-    <t>Thank you for attending the Corporate Conclave. We look forward to an insightful session with you. You can check the agenda for today on the left</t>
+    <t xml:space="preserve">A warm welcome to the School of Sciences Industry-Academia Conclave. Thank you for being part of this gathering. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Welcome to Christ University. Thanks for joining the Industry-Academia Conclave by the School of Sciences. We are happy to have you today. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">We are honored to welcome you to the Christ University Industry-Academia Conclave. Your presence enriches our event. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Greetings! We are delighted to have you join us for today's Industry-Academia Conclave at Christ University. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thank you for attending the Industry-Academia Conclave. We look forward to an insightful session with you. </t>
   </si>
 </sst>
 </file>
@@ -402,8 +402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" zoomScale="175" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -415,7 +415,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
@@ -425,7 +425,7 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>